<commit_message>
Agrego clase para metodo de Lopez
</commit_message>
<xml_diff>
--- a/temp/ConstantesEcuacionLopez.xlsx
+++ b/temp/ConstantesEcuacionLopez.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Control</t>
   </si>
@@ -56,19 +56,13 @@
     <t>PI</t>
   </si>
   <si>
-    <t>0.986</t>
-  </si>
-  <si>
-    <t>0.952</t>
-  </si>
-  <si>
-    <t>0.917</t>
-  </si>
-  <si>
-    <t>Z&amp;N</t>
-  </si>
-  <si>
-    <t>1.0</t>
+    <t>0,986</t>
+  </si>
+  <si>
+    <t>0,952</t>
+  </si>
+  <si>
+    <t>0,917</t>
   </si>
   <si>
     <t>PID</t>
@@ -78,13 +72,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="@" numFmtId="165"/>
   </numFmts>
   <fonts count="6">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -105,12 +99,14 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="12"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="12"/>
     </font>
@@ -185,7 +181,7 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="165" xfId="0">
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -206,10 +202,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="H12" activeCellId="0" pane="topLeft" sqref="A1:H12"/>
+      <selection activeCell="C2" activeCellId="0" pane="topLeft" sqref="C2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -356,123 +352,81 @@
       <c r="H7" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="8">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C8" s="4" t="n">
-        <v>0.909</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>17</v>
+        <v>1.435</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>0.921</v>
       </c>
       <c r="E8" s="4" t="n">
-        <v>3.333</v>
+        <v>1.139</v>
       </c>
       <c r="F8" s="4" t="n">
+        <v>0.749</v>
+      </c>
+      <c r="G8" s="4" t="n">
+        <v>0.482</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>1.13</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="9">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>1.495</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>0.945</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>0.917</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <v>0.771</v>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>0.56</v>
+      </c>
+      <c r="H9" s="4" t="n">
         <v>1</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="9">
-      <c r="A9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="4" t="n">
-        <v>1.435</v>
-      </c>
-      <c r="D9" s="4" t="n">
-        <v>0.921</v>
-      </c>
-      <c r="E9" s="4" t="n">
-        <v>1.139</v>
-      </c>
-      <c r="F9" s="4" t="n">
-        <v>0.749</v>
-      </c>
-      <c r="G9" s="4" t="n">
-        <v>0.482</v>
-      </c>
-      <c r="H9" s="4" t="n">
-        <v>1.13</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="10">
       <c r="A10" s="2"/>
       <c r="B10" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="4" t="n">
-        <v>1.495</v>
+        <v>1.357</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>0.945</v>
+        <v>0.947</v>
       </c>
       <c r="E10" s="4" t="n">
-        <v>0.917</v>
+        <v>1.176</v>
       </c>
       <c r="F10" s="4" t="n">
-        <v>0.771</v>
+        <v>0.738</v>
       </c>
       <c r="G10" s="4" t="n">
-        <v>0.56</v>
+        <v>0.381</v>
       </c>
       <c r="H10" s="4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="11">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="4" t="n">
-        <v>1.357</v>
-      </c>
-      <c r="D11" s="4" t="n">
-        <v>0.947</v>
-      </c>
-      <c r="E11" s="4" t="n">
-        <v>1.176</v>
-      </c>
-      <c r="F11" s="4" t="n">
-        <v>0.738</v>
-      </c>
-      <c r="G11" s="4" t="n">
-        <v>0.381</v>
-      </c>
-      <c r="H11" s="4" t="n">
         <v>0.99</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="12">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="4" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="D12" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="F12" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="H12" s="4" t="n">
-        <v>1</v>
-      </c>
-    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15"/>
@@ -495,13 +449,11 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>